<commit_message>
Updated Timesheet - Brindha
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-TimeSheet.xlsx
+++ b/Process/Timesheet/PTW-TimeSheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25301"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{688AC908-BD17-4F50-91EF-2E3F69B9A1C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F811F644-32A9-4696-A737-504537B0B2CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="27" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3832" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3822" uniqueCount="620">
   <si>
     <t>Resource Name</t>
   </si>
@@ -37027,10 +37027,10 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2B8ADE1-93B9-4EDE-A55C-8B6B4501AC81}">
-  <dimension ref="A1:Q141"/>
+  <dimension ref="A1:Q126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="A104" sqref="A104:F118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -39170,14 +39170,25 @@
       <c r="F103" s="108"/>
     </row>
     <row r="104" spans="1:9">
-      <c r="A104" s="143" t="s">
-        <v>19</v>
-      </c>
-      <c r="B104" s="136"/>
-      <c r="C104" s="136"/>
-      <c r="D104" s="137"/>
-      <c r="E104" s="137"/>
-      <c r="F104" s="137"/>
+      <c r="A104" s="145" t="s">
+        <v>339</v>
+      </c>
+      <c r="B104" s="115" t="s">
+        <v>557</v>
+      </c>
+      <c r="C104" s="107" t="s">
+        <v>290</v>
+      </c>
+      <c r="D104" s="108">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="E104" s="108">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="F104" s="108">
+        <f>E104-D104</f>
+        <v>6.9444444444444753E-3</v>
+      </c>
       <c r="H104" s="106" t="s">
         <v>291</v>
       </c>
@@ -39186,534 +39197,343 @@
       </c>
     </row>
     <row r="105" spans="1:9">
-      <c r="A105" s="143"/>
-      <c r="B105" s="136"/>
-      <c r="C105" s="136"/>
-      <c r="D105" s="137"/>
-      <c r="E105" s="137"/>
-      <c r="F105" s="137"/>
+      <c r="A105" s="145"/>
+      <c r="B105" s="115" t="s">
+        <v>614</v>
+      </c>
+      <c r="C105" s="107" t="s">
+        <v>290</v>
+      </c>
+      <c r="D105" s="108">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="E105" s="108">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="F105" s="108">
+        <f>E105-D105</f>
+        <v>8.3333333333333315E-2</v>
+      </c>
       <c r="H105" s="109" t="s">
         <v>290</v>
       </c>
       <c r="I105" s="108">
-        <f>SUMIFS(F102:F116, C102:C116,H105)</f>
-        <v>0</v>
+        <f>SUMIFS(F104:F116, C104:C116,H105)</f>
+        <v>0.28819444444444448</v>
       </c>
     </row>
     <row r="106" spans="1:9">
-      <c r="A106" s="143"/>
-      <c r="B106" s="136"/>
-      <c r="C106" s="136"/>
-      <c r="D106" s="137"/>
-      <c r="E106" s="137"/>
-      <c r="F106" s="137"/>
+      <c r="A106" s="145"/>
+      <c r="B106" s="107" t="s">
+        <v>301</v>
+      </c>
+      <c r="C106" s="107" t="s">
+        <v>299</v>
+      </c>
+      <c r="D106" s="108">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="E106" s="108">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="F106" s="108">
+        <f>E106-D106</f>
+        <v>2.083333333333337E-2</v>
+      </c>
       <c r="H106" s="109" t="s">
         <v>295</v>
       </c>
       <c r="I106" s="108">
-        <f>SUMIFS(F102:F116, C102:C116,H106)</f>
-        <v>0</v>
+        <f>SUMIFS(F104:F116, C104:C116,H106)</f>
+        <v>4.1666666666666741E-2</v>
       </c>
     </row>
     <row r="107" spans="1:9">
-      <c r="A107" s="143"/>
-      <c r="B107" s="136"/>
-      <c r="C107" s="136"/>
-      <c r="D107" s="137"/>
-      <c r="E107" s="137"/>
-      <c r="F107" s="137"/>
+      <c r="A107" s="145"/>
+      <c r="B107" s="107" t="s">
+        <v>615</v>
+      </c>
+      <c r="C107" s="107" t="s">
+        <v>290</v>
+      </c>
+      <c r="D107" s="108">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="E107" s="108">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="F107" s="108">
+        <f>E107-D107</f>
+        <v>7.6388888888888784E-2</v>
+      </c>
       <c r="H107" s="109" t="s">
         <v>297</v>
       </c>
       <c r="I107" s="108">
-        <f>SUMIFS(F102:F116, C102:C116,H107)</f>
+        <f>SUMIFS(F104:F116, C104:C116,H107)</f>
         <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:9">
-      <c r="A108" s="143"/>
-      <c r="B108" s="136"/>
-      <c r="C108" s="136"/>
-      <c r="D108" s="137"/>
-      <c r="E108" s="137"/>
-      <c r="F108" s="137"/>
+      <c r="A108" s="145"/>
+      <c r="B108" s="107" t="s">
+        <v>310</v>
+      </c>
+      <c r="C108" s="107" t="s">
+        <v>299</v>
+      </c>
+      <c r="D108" s="108">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="E108" s="108">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="F108" s="108">
+        <f>E108-D108</f>
+        <v>2.430555555555558E-2</v>
+      </c>
       <c r="H108" s="109" t="s">
         <v>300</v>
       </c>
       <c r="I108" s="108">
-        <f>SUMIFS(F102:F116, C102:C116,H108)</f>
-        <v>0</v>
+        <f>SUMIFS(F104:F116, C104:C116,H108)</f>
+        <v>1.7361111111111049E-2</v>
       </c>
     </row>
     <row r="109" spans="1:9">
-      <c r="A109" s="143"/>
-      <c r="B109" s="136"/>
-      <c r="C109" s="136"/>
-      <c r="D109" s="137"/>
-      <c r="E109" s="137"/>
-      <c r="F109" s="137"/>
+      <c r="A109" s="145"/>
+      <c r="B109" s="107" t="s">
+        <v>616</v>
+      </c>
+      <c r="C109" s="107" t="s">
+        <v>290</v>
+      </c>
+      <c r="D109" s="108">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="E109" s="108">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F109" s="108">
+        <f>E109-D109</f>
+        <v>1.0416666666666741E-2</v>
+      </c>
       <c r="H109" s="109" t="s">
         <v>302</v>
       </c>
       <c r="I109" s="108">
-        <f>SUMIFS(F102:F116, C102:C116,H109)</f>
-        <v>0</v>
+        <f>SUMIFS(F104:F116, C104:C116,H109)</f>
+        <v>6.2499999999999889E-2</v>
       </c>
     </row>
     <row r="110" spans="1:9">
-      <c r="A110" s="143"/>
-      <c r="B110" s="136"/>
-      <c r="C110" s="136"/>
-      <c r="D110" s="137"/>
-      <c r="E110" s="137"/>
-      <c r="F110" s="137"/>
+      <c r="A110" s="145"/>
+      <c r="B110" s="107" t="s">
+        <v>617</v>
+      </c>
+      <c r="C110" s="107" t="s">
+        <v>290</v>
+      </c>
+      <c r="D110" s="108">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E110" s="108">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="F110" s="108">
+        <f t="shared" ref="F110:F115" si="20">E110-D110</f>
+        <v>2.0833333333333259E-2</v>
+      </c>
       <c r="H110" s="109" t="s">
         <v>299</v>
       </c>
       <c r="I110" s="108">
-        <f>SUMIFS(F102:F116, C102:C116,H110)</f>
-        <v>0</v>
+        <f>SUMIFS(F104:F116, C104:C116,H110)</f>
+        <v>6.597222222222221E-2</v>
       </c>
     </row>
     <row r="111" spans="1:9">
-      <c r="A111" s="143"/>
-      <c r="B111" s="136"/>
-      <c r="C111" s="136"/>
-      <c r="D111" s="137"/>
-      <c r="E111" s="137"/>
-      <c r="F111" s="137"/>
+      <c r="A111" s="145"/>
+      <c r="B111" s="107" t="s">
+        <v>294</v>
+      </c>
+      <c r="C111" s="107" t="s">
+        <v>302</v>
+      </c>
+      <c r="D111" s="108">
+        <v>0.60763888888888895</v>
+      </c>
+      <c r="E111" s="108">
+        <v>0.64930555555555558</v>
+      </c>
+      <c r="F111" s="108">
+        <f t="shared" si="20"/>
+        <v>4.166666666666663E-2</v>
+      </c>
       <c r="H111" s="105" t="s">
         <v>305</v>
       </c>
       <c r="I111" s="106">
-        <f t="shared" ref="I111" si="20">SUM(I105:I110)</f>
-        <v>0</v>
+        <f t="shared" ref="I111" si="21">SUM(I105:I110)</f>
+        <v>0.47569444444444436</v>
       </c>
     </row>
     <row r="112" spans="1:9">
-      <c r="A112" s="143"/>
-      <c r="B112" s="136"/>
-      <c r="C112" s="136"/>
-      <c r="D112" s="137"/>
-      <c r="E112" s="137"/>
-      <c r="F112" s="137"/>
+      <c r="A112" s="145"/>
+      <c r="B112" s="111" t="s">
+        <v>314</v>
+      </c>
+      <c r="C112" s="111" t="s">
+        <v>300</v>
+      </c>
+      <c r="D112" s="112">
+        <v>0.64930555555555558</v>
+      </c>
+      <c r="E112" s="112">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F112" s="108">
+        <f t="shared" si="20"/>
+        <v>1.7361111111111049E-2</v>
+      </c>
       <c r="I112" s="110"/>
     </row>
     <row r="113" spans="1:9">
-      <c r="A113" s="143"/>
-      <c r="B113" s="136"/>
-      <c r="C113" s="136"/>
-      <c r="D113" s="137"/>
-      <c r="E113" s="137"/>
-      <c r="F113" s="137"/>
+      <c r="A113" s="145"/>
+      <c r="B113" s="107" t="s">
+        <v>509</v>
+      </c>
+      <c r="C113" s="107" t="s">
+        <v>295</v>
+      </c>
+      <c r="D113" s="108">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E113" s="108">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F113" s="108">
+        <f t="shared" si="20"/>
+        <v>4.1666666666666741E-2</v>
+      </c>
       <c r="I113" s="110"/>
     </row>
     <row r="114" spans="1:9">
-      <c r="A114" s="143"/>
-      <c r="B114" s="136"/>
-      <c r="C114" s="136"/>
-      <c r="D114" s="137"/>
-      <c r="E114" s="137"/>
-      <c r="F114" s="137"/>
+      <c r="A114" s="145"/>
+      <c r="B114" s="111" t="s">
+        <v>303</v>
+      </c>
+      <c r="C114" s="111" t="s">
+        <v>299</v>
+      </c>
+      <c r="D114" s="108">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E114" s="112">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="F114" s="112">
+        <f t="shared" si="20"/>
+        <v>2.0833333333333259E-2</v>
+      </c>
     </row>
     <row r="115" spans="1:9">
-      <c r="A115" s="143"/>
-      <c r="B115" s="136"/>
-      <c r="C115" s="136"/>
-      <c r="D115" s="137"/>
-      <c r="E115" s="137"/>
-      <c r="F115" s="137"/>
+      <c r="A115" s="145"/>
+      <c r="B115" s="107" t="s">
+        <v>618</v>
+      </c>
+      <c r="C115" s="111" t="s">
+        <v>290</v>
+      </c>
+      <c r="D115" s="108">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="E115" s="108">
+        <v>0.81944444444444453</v>
+      </c>
+      <c r="F115" s="114">
+        <f t="shared" si="20"/>
+        <v>9.0277777777777901E-2</v>
+      </c>
     </row>
     <row r="116" spans="1:9">
-      <c r="A116" s="143"/>
-      <c r="B116" s="136"/>
-      <c r="C116" s="136"/>
-      <c r="D116" s="137"/>
-      <c r="E116" s="137"/>
-      <c r="F116" s="137"/>
+      <c r="A116" s="145"/>
+      <c r="B116" s="107" t="s">
+        <v>563</v>
+      </c>
+      <c r="C116" s="111" t="s">
+        <v>302</v>
+      </c>
+      <c r="D116" s="108">
+        <v>0.81944444444444453</v>
+      </c>
+      <c r="E116" s="108">
+        <v>0.84027777777777779</v>
+      </c>
+      <c r="F116" s="114">
+        <f t="shared" ref="F111:F174" si="22">E116-D116</f>
+        <v>2.0833333333333259E-2</v>
+      </c>
     </row>
     <row r="117" spans="1:9">
-      <c r="A117" s="143"/>
-      <c r="B117" s="136"/>
-      <c r="C117" s="136"/>
-      <c r="D117" s="137"/>
-      <c r="E117" s="137"/>
-      <c r="F117" s="137"/>
+      <c r="A117" s="145"/>
+      <c r="B117" s="116" t="s">
+        <v>619</v>
+      </c>
+      <c r="C117" s="111" t="s">
+        <v>290</v>
+      </c>
+      <c r="D117" s="112">
+        <v>0.84722222222222221</v>
+      </c>
+      <c r="E117" s="112">
+        <v>0.86111111111111116</v>
+      </c>
+      <c r="F117" s="112">
+        <f>E117-D117</f>
+        <v>1.3888888888888951E-2</v>
+      </c>
     </row>
     <row r="118" spans="1:9">
-      <c r="A118" s="144"/>
-      <c r="B118" s="136"/>
-      <c r="C118" s="136"/>
-      <c r="D118" s="137"/>
-      <c r="E118" s="137"/>
-      <c r="F118" s="137"/>
+      <c r="A118" s="145"/>
+      <c r="B118" s="117"/>
+      <c r="C118" s="113"/>
+      <c r="D118" s="114"/>
+      <c r="E118" s="114"/>
+      <c r="F118" s="114"/>
     </row>
     <row r="119" spans="1:9">
-      <c r="A119" s="145" t="s">
-        <v>339</v>
-      </c>
-      <c r="B119" s="115" t="s">
-        <v>557</v>
-      </c>
-      <c r="C119" s="107" t="s">
-        <v>290</v>
-      </c>
-      <c r="D119" s="108">
-        <v>0.3611111111111111</v>
-      </c>
-      <c r="E119" s="108">
-        <v>0.36805555555555558</v>
-      </c>
-      <c r="F119" s="108">
-        <f>E119-D119</f>
-        <v>6.9444444444444753E-3</v>
-      </c>
-      <c r="H119" s="106" t="s">
-        <v>291</v>
-      </c>
-      <c r="I119" s="106" t="s">
-        <v>292</v>
-      </c>
+      <c r="A119" s="123"/>
+      <c r="H119" s="122"/>
+      <c r="I119" s="122"/>
     </row>
     <row r="120" spans="1:9">
-      <c r="A120" s="145"/>
-      <c r="B120" s="115" t="s">
-        <v>614</v>
-      </c>
-      <c r="C120" s="107" t="s">
-        <v>290</v>
-      </c>
-      <c r="D120" s="108">
-        <v>0.36805555555555558</v>
-      </c>
-      <c r="E120" s="108">
-        <v>0.4513888888888889</v>
-      </c>
-      <c r="F120" s="108">
-        <f>E120-D120</f>
-        <v>8.3333333333333315E-2</v>
-      </c>
-      <c r="H120" s="109" t="s">
-        <v>290</v>
-      </c>
-      <c r="I120" s="108">
-        <f>SUMIFS(F117:F131, C117:C131,H120)</f>
-        <v>0.28819444444444448</v>
-      </c>
+      <c r="A120" s="123"/>
+      <c r="I120" s="110"/>
     </row>
     <row r="121" spans="1:9">
-      <c r="A121" s="145"/>
-      <c r="B121" s="107" t="s">
-        <v>301</v>
-      </c>
-      <c r="C121" s="107" t="s">
-        <v>299</v>
-      </c>
-      <c r="D121" s="108">
-        <v>0.4513888888888889</v>
-      </c>
-      <c r="E121" s="108">
-        <v>0.47222222222222227</v>
-      </c>
-      <c r="F121" s="108">
-        <f>E121-D121</f>
-        <v>2.083333333333337E-2</v>
-      </c>
-      <c r="H121" s="109" t="s">
-        <v>295</v>
-      </c>
-      <c r="I121" s="108">
-        <f>SUMIFS(F117:F131, C117:C131,H121)</f>
-        <v>4.1666666666666741E-2</v>
-      </c>
+      <c r="A121" s="123"/>
+      <c r="I121" s="110"/>
     </row>
     <row r="122" spans="1:9">
-      <c r="A122" s="145"/>
-      <c r="B122" s="107" t="s">
-        <v>615</v>
-      </c>
-      <c r="C122" s="107" t="s">
-        <v>290</v>
-      </c>
-      <c r="D122" s="108">
-        <v>0.47222222222222227</v>
-      </c>
-      <c r="E122" s="108">
-        <v>0.54861111111111105</v>
-      </c>
-      <c r="F122" s="108">
-        <f>E122-D122</f>
-        <v>7.6388888888888784E-2</v>
-      </c>
-      <c r="H122" s="109" t="s">
-        <v>297</v>
-      </c>
-      <c r="I122" s="108">
-        <f>SUMIFS(F117:F131, C117:C131,H122)</f>
-        <v>0</v>
-      </c>
+      <c r="A122" s="123"/>
     </row>
     <row r="123" spans="1:9">
-      <c r="A123" s="145"/>
-      <c r="B123" s="107" t="s">
-        <v>310</v>
-      </c>
-      <c r="C123" s="107" t="s">
-        <v>299</v>
-      </c>
-      <c r="D123" s="108">
-        <v>0.54861111111111105</v>
-      </c>
-      <c r="E123" s="108">
-        <v>0.57291666666666663</v>
-      </c>
-      <c r="F123" s="108">
-        <f>E123-D123</f>
-        <v>2.430555555555558E-2</v>
-      </c>
-      <c r="H123" s="109" t="s">
-        <v>300</v>
-      </c>
-      <c r="I123" s="108">
-        <f>SUMIFS(F117:F131, C117:C131,H123)</f>
-        <v>1.7361111111111049E-2</v>
-      </c>
+      <c r="A123" s="123"/>
     </row>
     <row r="124" spans="1:9">
-      <c r="A124" s="145"/>
-      <c r="B124" s="107" t="s">
-        <v>616</v>
-      </c>
-      <c r="C124" s="107" t="s">
-        <v>290</v>
-      </c>
-      <c r="D124" s="108">
-        <v>0.57291666666666663</v>
-      </c>
-      <c r="E124" s="108">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="F124" s="108">
-        <f>E124-D124</f>
-        <v>1.0416666666666741E-2</v>
-      </c>
-      <c r="H124" s="109" t="s">
-        <v>302</v>
-      </c>
-      <c r="I124" s="108">
-        <f>SUMIFS(F117:F131, C117:C131,H124)</f>
-        <v>6.2499999999999889E-2</v>
-      </c>
+      <c r="A124" s="123"/>
     </row>
     <row r="125" spans="1:9">
-      <c r="A125" s="145"/>
-      <c r="B125" s="107" t="s">
-        <v>617</v>
-      </c>
-      <c r="C125" s="107" t="s">
-        <v>290</v>
-      </c>
-      <c r="D125" s="108">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="E125" s="108">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="F125" s="108">
-        <f t="shared" ref="F125:F130" si="21">E125-D125</f>
-        <v>2.0833333333333259E-2</v>
-      </c>
-      <c r="H125" s="109" t="s">
-        <v>299</v>
-      </c>
-      <c r="I125" s="108">
-        <f>SUMIFS(F117:F131, C117:C131,H125)</f>
-        <v>6.597222222222221E-2</v>
-      </c>
+      <c r="A125" s="123"/>
     </row>
     <row r="126" spans="1:9">
-      <c r="A126" s="145"/>
-      <c r="B126" s="107" t="s">
-        <v>294</v>
-      </c>
-      <c r="C126" s="107" t="s">
-        <v>302</v>
-      </c>
-      <c r="D126" s="108">
-        <v>0.60763888888888895</v>
-      </c>
-      <c r="E126" s="108">
-        <v>0.64930555555555558</v>
-      </c>
-      <c r="F126" s="108">
-        <f t="shared" si="21"/>
-        <v>4.166666666666663E-2</v>
-      </c>
-      <c r="H126" s="105" t="s">
-        <v>305</v>
-      </c>
-      <c r="I126" s="106">
-        <f t="shared" ref="I126" si="22">SUM(I120:I125)</f>
-        <v>0.47569444444444436</v>
-      </c>
-    </row>
-    <row r="127" spans="1:9">
-      <c r="A127" s="145"/>
-      <c r="B127" s="111" t="s">
-        <v>314</v>
-      </c>
-      <c r="C127" s="111" t="s">
-        <v>300</v>
-      </c>
-      <c r="D127" s="112">
-        <v>0.64930555555555558</v>
-      </c>
-      <c r="E127" s="112">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="F127" s="108">
-        <f t="shared" si="21"/>
-        <v>1.7361111111111049E-2</v>
-      </c>
-      <c r="I127" s="110"/>
-    </row>
-    <row r="128" spans="1:9">
-      <c r="A128" s="145"/>
-      <c r="B128" s="107" t="s">
-        <v>509</v>
-      </c>
-      <c r="C128" s="107" t="s">
-        <v>295</v>
-      </c>
-      <c r="D128" s="108">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="E128" s="108">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="F128" s="108">
-        <f t="shared" si="21"/>
-        <v>4.1666666666666741E-2</v>
-      </c>
-      <c r="I128" s="110"/>
-    </row>
-    <row r="129" spans="1:9">
-      <c r="A129" s="145"/>
-      <c r="B129" s="111" t="s">
-        <v>303</v>
-      </c>
-      <c r="C129" s="111" t="s">
-        <v>299</v>
-      </c>
-      <c r="D129" s="108">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="E129" s="112">
-        <v>0.72916666666666663</v>
-      </c>
-      <c r="F129" s="112">
-        <f t="shared" si="21"/>
-        <v>2.0833333333333259E-2</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9">
-      <c r="A130" s="145"/>
-      <c r="B130" s="107" t="s">
-        <v>618</v>
-      </c>
-      <c r="C130" s="111" t="s">
-        <v>290</v>
-      </c>
-      <c r="D130" s="108">
-        <v>0.72916666666666663</v>
-      </c>
-      <c r="E130" s="108">
-        <v>0.81944444444444453</v>
-      </c>
-      <c r="F130" s="114">
-        <f t="shared" si="21"/>
-        <v>9.0277777777777901E-2</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9">
-      <c r="A131" s="145"/>
-      <c r="B131" s="107" t="s">
-        <v>563</v>
-      </c>
-      <c r="C131" s="111" t="s">
-        <v>302</v>
-      </c>
-      <c r="D131" s="108">
-        <v>0.81944444444444453</v>
-      </c>
-      <c r="E131" s="108">
-        <v>0.84027777777777779</v>
-      </c>
-      <c r="F131" s="114">
-        <f t="shared" ref="F126:F189" si="23">E131-D131</f>
-        <v>2.0833333333333259E-2</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9">
-      <c r="A132" s="145"/>
-      <c r="B132" s="116" t="s">
-        <v>619</v>
-      </c>
-      <c r="C132" s="111" t="s">
-        <v>290</v>
-      </c>
-      <c r="D132" s="112">
-        <v>0.84722222222222221</v>
-      </c>
-      <c r="E132" s="112">
-        <v>0.86111111111111116</v>
-      </c>
-      <c r="F132" s="112">
-        <f>E132-D132</f>
-        <v>1.3888888888888951E-2</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9">
-      <c r="A133" s="145"/>
-      <c r="B133" s="117"/>
-      <c r="C133" s="113"/>
-      <c r="D133" s="114"/>
-      <c r="E133" s="114"/>
-      <c r="F133" s="114"/>
-    </row>
-    <row r="134" spans="1:9">
-      <c r="A134" s="123"/>
-      <c r="H134" s="122"/>
-      <c r="I134" s="122"/>
-    </row>
-    <row r="135" spans="1:9">
-      <c r="A135" s="123"/>
-      <c r="I135" s="110"/>
-    </row>
-    <row r="136" spans="1:9">
-      <c r="A136" s="123"/>
-      <c r="I136" s="110"/>
-    </row>
-    <row r="137" spans="1:9">
-      <c r="A137" s="123"/>
-    </row>
-    <row r="138" spans="1:9">
-      <c r="A138" s="123"/>
-    </row>
-    <row r="139" spans="1:9">
-      <c r="A139" s="123"/>
-    </row>
-    <row r="140" spans="1:9">
-      <c r="A140" s="123"/>
-    </row>
-    <row r="141" spans="1:9">
-      <c r="A141" s="123"/>
+      <c r="A126" s="123"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="8">
     <mergeCell ref="A89:A103"/>
     <mergeCell ref="A104:A118"/>
-    <mergeCell ref="A119:A133"/>
     <mergeCell ref="A2:A16"/>
     <mergeCell ref="A17:A28"/>
     <mergeCell ref="A29:A43"/>
@@ -39721,7 +39541,7 @@
     <mergeCell ref="A58:A73"/>
     <mergeCell ref="A74:A88"/>
   </mergeCells>
-  <conditionalFormatting sqref="I3 I18 I30 I45 I59 I75 I90 I105">
+  <conditionalFormatting sqref="I3 I18 I30 I45 I59 I75 I90">
     <cfRule type="cellIs" dxfId="25" priority="25" operator="greaterThan">
       <formula>0.25</formula>
     </cfRule>
@@ -39729,7 +39549,7 @@
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4 I19 I31 I46 I60 I76 I91 I106">
+  <conditionalFormatting sqref="I4 I19 I31 I46 I60 I76 I91">
     <cfRule type="cellIs" dxfId="23" priority="22" operator="lessThan">
       <formula>0.0416666666666667</formula>
     </cfRule>
@@ -39740,7 +39560,7 @@
       <formula>0.0416666666666667</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5 I20 I32 I47 I61 I77 I92 I107">
+  <conditionalFormatting sqref="I5 I20 I32 I47 I61 I77 I92">
     <cfRule type="cellIs" dxfId="20" priority="20" operator="lessThan">
       <formula>0.0833333333333333</formula>
     </cfRule>
@@ -39748,7 +39568,7 @@
       <formula>0.0833333333333333</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I6 I21 I33 I48 I62 I78 I93 I108">
+  <conditionalFormatting sqref="I6 I21 I33 I48 I62 I78 I93">
     <cfRule type="cellIs" dxfId="18" priority="18" operator="lessThan">
       <formula>0.0416666666666667</formula>
     </cfRule>
@@ -39756,7 +39576,7 @@
       <formula>0.0416666666666667</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7 I22 I34 I49 I63 I79 I94 I109">
+  <conditionalFormatting sqref="I7 I22 I34 I49 I63 I79 I94">
     <cfRule type="cellIs" dxfId="16" priority="16" operator="lessThan">
       <formula>0.0416666666666667</formula>
     </cfRule>
@@ -39764,7 +39584,7 @@
       <formula>0.0416666666666667</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I8 I23 I35 I50 I80 I95 I110 I64">
+  <conditionalFormatting sqref="I8 I23 I35 I50 I80 I95 I64">
     <cfRule type="cellIs" dxfId="14" priority="14" operator="lessThan">
       <formula>0.0625</formula>
     </cfRule>
@@ -39772,7 +39592,7 @@
       <formula>0.0625</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I120">
+  <conditionalFormatting sqref="I105">
     <cfRule type="cellIs" dxfId="12" priority="12" operator="greaterThan">
       <formula>0.25</formula>
     </cfRule>
@@ -39780,7 +39600,7 @@
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I121">
+  <conditionalFormatting sqref="I106">
     <cfRule type="cellIs" dxfId="10" priority="9" operator="lessThan">
       <formula>0.0416666666666667</formula>
     </cfRule>
@@ -39791,7 +39611,7 @@
       <formula>0.0416666666666667</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I122">
+  <conditionalFormatting sqref="I107">
     <cfRule type="cellIs" dxfId="7" priority="7" operator="lessThan">
       <formula>0.0833333333333333</formula>
     </cfRule>
@@ -39799,7 +39619,7 @@
       <formula>0.0833333333333333</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I123">
+  <conditionalFormatting sqref="I108">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="lessThan">
       <formula>0.0416666666666667</formula>
     </cfRule>
@@ -39807,7 +39627,7 @@
       <formula>0.0416666666666667</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I124">
+  <conditionalFormatting sqref="I109">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
       <formula>0.0416666666666667</formula>
     </cfRule>
@@ -39815,7 +39635,7 @@
       <formula>0.0416666666666667</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I125">
+  <conditionalFormatting sqref="I110">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0.0625</formula>
     </cfRule>
@@ -39824,7 +39644,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C139" xr:uid="{4B34E0AC-E4AC-4BE5-8464-7DC5384CA00B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C124" xr:uid="{4B34E0AC-E4AC-4BE5-8464-7DC5384CA00B}">
       <formula1>$Q$1:$Q$7</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>